<commit_message>
several fixes for appium integration
</commit_message>
<xml_diff>
--- a/examples/AppTestRunDefinition.xlsx
+++ b/examples/AppTestRunDefinition.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE761055-0542-E34C-A6AE-198852666E8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540" activeTab="3"/>
+    <workbookView xWindow="2600" yWindow="5160" windowWidth="28800" windowHeight="12540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestRun" sheetId="1" r:id="rId1"/>
@@ -19,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Bernhard Buhl</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Attribute</t>
   </si>
@@ -255,23 +261,20 @@
   </si>
   <si>
     <t>//android.widget.Button[@content-desc="equals"]</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -279,7 +282,7 @@
       <u/>
       <sz val="12"/>
       <color rgb="FF800080"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -297,154 +300,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -461,201 +321,15 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -663,313 +337,30 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1227,24 +618,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1252,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1261,107 +652,101 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83333333333333" customWidth="1"/>
-    <col min="2" max="2" width="29.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="12.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1381,7 +766,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1397,39 +782,37 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
-    <col min="5" max="5" width="20.25" customWidth="1"/>
-    <col min="6" max="6" width="19.125" customWidth="1"/>
-    <col min="8" max="8" width="22.375" customWidth="1"/>
-    <col min="9" max="9" width="20.25" customWidth="1"/>
-    <col min="10" max="10" width="23.75" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1473,7 +856,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1489,31 +872,32 @@
       <c r="E2" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="54.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="54.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1530,7 +914,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1545,32 +929,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="7.16666666666667" customWidth="1"/>
-    <col min="3" max="3" width="7.33333333333333" customWidth="1"/>
-    <col min="4" max="4" width="23.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="54.3333333333333" customWidth="1"/>
-    <col min="8" max="8" width="35.125" customWidth="1"/>
+    <col min="7" max="7" width="54.33203125" customWidth="1"/>
+    <col min="8" max="8" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1611,7 +993,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1640,7 +1022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1664,8 +1046,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>